<commit_message>
hopefully it will work this time
</commit_message>
<xml_diff>
--- a/data/results.xlsx
+++ b/data/results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,6 +528,106 @@
           <t>question_2_selections</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>question_3_hint_used</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>question_3_tries_taken</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>question_3_correct</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>question_3_selections</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>question_4_hint_used</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>question_4_tries_taken</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>question_4_correct</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>question_4_selections</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>question_5_hint_used</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>question_5_tries_taken</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>question_5_correct</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>question_5_selections</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>question_6_hint_used</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>question_6_tries_taken</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>question_6_correct</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>question_6_selections</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>question_7_hint_used</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>question_7_tries_taken</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>question_7_correct</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>question_7_selections</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -592,6 +692,128 @@
           <t>0,</t>
         </is>
       </c>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Autonomous Vehicle</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45873.12718336806</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45873.12720300926</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1697</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>